<commit_message>
fix: companies exported data
</commit_message>
<xml_diff>
--- a/posts.xlsx
+++ b/posts.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>post_id</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>post_name</t>
+          <t>name</t>
         </is>
       </c>
     </row>

</xml_diff>